<commit_message>
extra ex ch. 6
</commit_message>
<xml_diff>
--- a/shapes.xlsx
+++ b/shapes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4545" yWindow="0" windowWidth="27285" windowHeight="12285" activeTab="5"/>
+    <workbookView xWindow="6060" yWindow="0" windowWidth="27285" windowHeight="12285" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dataset1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="dataset5" sheetId="5" r:id="rId5"/>
     <sheet name="dataset6" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dataset3!$A$1:$B$372</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -367,7 +370,7 @@
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +832,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1245,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B372"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2784,7 +2789,7 @@
         <v>8</v>
       </c>
       <c r="B192">
-        <v>116.5</v>
+        <v>116</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3632,7 +3637,7 @@
         <v>10.9</v>
       </c>
       <c r="B298">
-        <v>63.5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
@@ -3680,7 +3685,7 @@
         <v>11.3</v>
       </c>
       <c r="B304">
-        <v>107.5</v>
+        <v>107</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -3904,7 +3909,7 @@
         <v>13.4</v>
       </c>
       <c r="B332">
-        <v>206.5</v>
+        <v>206</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
@@ -3984,7 +3989,7 @@
         <v>15.7</v>
       </c>
       <c r="B342">
-        <v>227.7</v>
+        <v>228</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
@@ -4000,7 +4005,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="B344">
-        <v>142.5</v>
+        <v>143</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
@@ -4228,6 +4233,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B372"/>
   <sortState ref="A2:B372">
     <sortCondition ref="A2:A372"/>
   </sortState>
@@ -8892,7 +8898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>